<commit_message>
Included push sum excel into project2-analysis.xls
</commit_message>
<xml_diff>
--- a/project2-analysis.xlsx
+++ b/project2-analysis.xlsx
@@ -15,6 +15,9 @@
     <sheet name="Gossip" sheetId="1" r:id="rId1"/>
     <sheet name="Failure Model" sheetId="3" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>Line</t>
   </si>
@@ -81,12 +84,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -95,6 +101,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF840001"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -612,11 +623,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1097458112"/>
-        <c:axId val="-1097454384"/>
+        <c:axId val="-1053295648"/>
+        <c:axId val="-1053292016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1097458112"/>
+        <c:axId val="-1053295648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,12 +728,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1097454384"/>
+        <c:crossAx val="-1053292016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1097454384"/>
+        <c:axId val="-1053292016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -836,7 +847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1097458112"/>
+        <c:crossAx val="-1053295648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -950,88 +961,69 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t> Full Spread %</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.110390118051755"/>
+          <c:y val="0.213370901639344"/>
+          <c:w val="0.889570791963099"/>
+          <c:h val="0.699965846994536"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>0</c:v>
+            <c:v>Full</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>'Failure Model'!$B$18:$B$22</c:f>
+              <c:f>Gossip!$B$16:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1052,51 +1044,80 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>'Failure Model'!$C$18:$C$22</c:f>
+              <c:f>Gossip!$C$16:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>97.0</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>99.66</c:v>
+                  <c:v>65.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.2</c:v>
+                  <c:v>340.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.62</c:v>
+                  <c:v>488.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>99.3</c:v>
+                  <c:v>716.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>10%</c:v>
+            <c:v>Line</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>'Failure Model'!$B$18:$B$22</c:f>
+              <c:f>Gossip!$B$16:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1117,51 +1138,80 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>'Failure Model'!$D$18:$D$22</c:f>
+              <c:f>Gossip!$D$16:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>88.0</c:v>
+                  <c:v>104.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.67</c:v>
+                  <c:v>560.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89.6</c:v>
+                  <c:v>1603.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89.62</c:v>
+                  <c:v>5308.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.1</c:v>
+                  <c:v>10383.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>20%</c:v>
+            <c:v>2D</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>'Failure Model'!$B$18:$B$22</c:f>
+              <c:f>Gossip!$B$16:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1182,31 +1232,126 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>'Failure Model'!$E$18:$E$22</c:f>
+              <c:f>Gossip!$E$16:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>80.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79.33</c:v>
+                  <c:v>83.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79.6</c:v>
+                  <c:v>368.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79.125</c:v>
+                  <c:v>504.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.7</c:v>
+                  <c:v>595.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Imp2D</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="840001"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Gossip!$B$16:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Gossip!$F$16:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>295.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1216,19 +1361,86 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-1096302096"/>
-        <c:axId val="-1171882416"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-1096302096"/>
+        <c:axId val="-1128803536"/>
+        <c:axId val="-1097971648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1128803536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1236,9 +1448,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1252,9 +1463,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1265,18 +1475,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1171882416"/>
+        <c:crossAx val="-1097971648"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="-1171882416"/>
+        <c:axId val="-1097971648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100.0"/>
+          <c:max val="8000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1284,9 +1491,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1294,15 +1502,74 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Convergence time in   milliseconds
+</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1313,9 +1580,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1326,9 +1592,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1096302096"/>
+        <c:crossAx val="-1128803536"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1339,7 +1605,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1356,9 +1622,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1370,17 +1635,20 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1442,20 +1710,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t> Line</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Spread %</a:t>
+              <a:t> Full Spread %</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1510,7 +1769,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Failure Model'!$G$18:$G$22</c:f>
+              <c:f>'Failure Model'!$B$18:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1534,24 +1793,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Failure Model'!$H$18:$H$22</c:f>
+              <c:f>'Failure Model'!$C$18:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>98.0</c:v>
+                  <c:v>97.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>99.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.8</c:v>
+                  <c:v>98.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.875</c:v>
+                  <c:v>99.62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56.8</c:v>
+                  <c:v>99.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1575,7 +1834,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Failure Model'!$G$18:$G$22</c:f>
+              <c:f>'Failure Model'!$B$18:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1599,24 +1858,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Failure Model'!$I$18:$I$22</c:f>
+              <c:f>'Failure Model'!$D$18:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6.0</c:v>
+                  <c:v>88.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.33</c:v>
+                  <c:v>88.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8</c:v>
+                  <c:v>89.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.125</c:v>
+                  <c:v>89.62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>88.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1640,7 +1899,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Failure Model'!$G$18:$G$22</c:f>
+              <c:f>'Failure Model'!$B$18:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1664,24 +1923,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Failure Model'!$J$18:$J$22</c:f>
+              <c:f>'Failure Model'!$E$18:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.66</c:v>
+                  <c:v>79.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8</c:v>
+                  <c:v>79.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>79.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2</c:v>
+                  <c:v>79.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1697,11 +1956,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1090758768"/>
-        <c:axId val="-1056411520"/>
+        <c:axId val="-1053747440"/>
+        <c:axId val="-1053608496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1090758768"/>
+        <c:axId val="-1053747440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +2003,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1056411520"/>
+        <c:crossAx val="-1053608496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1752,7 +2011,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1056411520"/>
+        <c:axId val="-1053608496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1805,7 +2064,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1090758768"/>
+        <c:crossAx val="-1053747440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1819,7 +2078,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1921,12 +2179,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t> 2D Spread %</a:t>
+              <a:t> Line</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Spread %</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1981,7 +2246,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Failure Model'!$B$26:$B$30</c:f>
+              <c:f>'Failure Model'!$G$18:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2005,7 +2270,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Failure Model'!$C$26:$C$30</c:f>
+              <c:f>'Failure Model'!$H$18:$H$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2013,16 +2278,16 @@
                   <c:v>98.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.66</c:v>
+                  <c:v>99.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.4</c:v>
+                  <c:v>99.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.25</c:v>
+                  <c:v>99.875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>99.3</c:v>
+                  <c:v>56.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2046,7 +2311,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Failure Model'!$B$26:$B$30</c:f>
+              <c:f>'Failure Model'!$G$18:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2070,24 +2335,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Failure Model'!$D$26:$D$30</c:f>
+              <c:f>'Failure Model'!$I$18:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>89.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.33</c:v>
+                  <c:v>8.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.6</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89.25</c:v>
+                  <c:v>1.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.3</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2111,7 +2376,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Failure Model'!$B$26:$B$30</c:f>
+              <c:f>'Failure Model'!$G$18:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2135,24 +2400,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Failure Model'!$E$26:$E$30</c:f>
+              <c:f>'Failure Model'!$J$18:$J$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>78.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.33</c:v>
+                  <c:v>3.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.6</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79.5</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.6</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2168,11 +2433,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1090641712"/>
-        <c:axId val="-1090639936"/>
+        <c:axId val="-1051447024"/>
+        <c:axId val="-1051444704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1090641712"/>
+        <c:axId val="-1051447024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2215,7 +2480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1090639936"/>
+        <c:crossAx val="-1051444704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2223,7 +2488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1090639936"/>
+        <c:axId val="-1051444704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2276,7 +2541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1090641712"/>
+        <c:crossAx val="-1051447024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2290,7 +2555,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2392,12 +2656,480 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t> 2D Spread %</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Failure Model'!$B$26:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Failure Model'!$C$26:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>10%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Failure Model'!$B$26:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Failure Model'!$D$26:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>20%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Failure Model'!$B$26:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Failure Model'!$E$26:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1051139696"/>
+        <c:axId val="-1051137376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1051139696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1051137376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1051137376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1051139696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t> Imp 2D Spread %</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2639,11 +3371,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1056243360"/>
-        <c:axId val="-1056241312"/>
+        <c:axId val="-1051106496"/>
+        <c:axId val="-1091037104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1056243360"/>
+        <c:axId val="-1051106496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2686,7 +3418,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1056241312"/>
+        <c:crossAx val="-1091037104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2694,7 +3426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1056241312"/>
+        <c:axId val="-1091037104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2747,7 +3479,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1056243360"/>
+        <c:crossAx val="-1051106496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2761,7 +3493,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3025,6 +3756,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -3522,6 +4293,544 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4024,7 +5333,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4527,7 +5836,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5030,7 +6339,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5537,16 +6846,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5560,6 +6869,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5699,6 +7040,107 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Gossip"/>
+      <sheetName val="Failure Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="B4">
+            <v>100</v>
+          </cell>
+          <cell r="C4">
+            <v>41</v>
+          </cell>
+          <cell r="D4">
+            <v>104</v>
+          </cell>
+          <cell r="E4">
+            <v>49</v>
+          </cell>
+          <cell r="F4">
+            <v>32</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>300</v>
+          </cell>
+          <cell r="C5">
+            <v>65</v>
+          </cell>
+          <cell r="D5">
+            <v>560</v>
+          </cell>
+          <cell r="E5">
+            <v>83</v>
+          </cell>
+          <cell r="F5">
+            <v>44</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>500</v>
+          </cell>
+          <cell r="C6">
+            <v>340</v>
+          </cell>
+          <cell r="D6">
+            <v>1603</v>
+          </cell>
+          <cell r="E6">
+            <v>368</v>
+          </cell>
+          <cell r="F6">
+            <v>142</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>800</v>
+          </cell>
+          <cell r="C7">
+            <v>488</v>
+          </cell>
+          <cell r="D7">
+            <v>5308</v>
+          </cell>
+          <cell r="E7">
+            <v>504</v>
+          </cell>
+          <cell r="F7">
+            <v>125</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>1000</v>
+          </cell>
+          <cell r="C8">
+            <v>716</v>
+          </cell>
+          <cell r="D8">
+            <v>10383</v>
+          </cell>
+          <cell r="E8">
+            <v>595</v>
+          </cell>
+          <cell r="F8">
+            <v>295</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5962,10 +7404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F8"/>
+  <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6077,6 +7519,115 @@
       </c>
       <c r="F8" s="1">
         <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="3">
+        <v>100</v>
+      </c>
+      <c r="C16" s="3">
+        <v>41</v>
+      </c>
+      <c r="D16" s="3">
+        <v>104</v>
+      </c>
+      <c r="E16" s="3">
+        <v>49</v>
+      </c>
+      <c r="F16" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="3">
+        <v>300</v>
+      </c>
+      <c r="C17" s="3">
+        <v>65</v>
+      </c>
+      <c r="D17" s="3">
+        <v>560</v>
+      </c>
+      <c r="E17" s="3">
+        <v>83</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="3">
+        <v>500</v>
+      </c>
+      <c r="C18" s="3">
+        <v>340</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1603</v>
+      </c>
+      <c r="E18" s="3">
+        <v>368</v>
+      </c>
+      <c r="F18" s="3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="3">
+        <v>800</v>
+      </c>
+      <c r="C19" s="3">
+        <v>488</v>
+      </c>
+      <c r="D19" s="3">
+        <v>5308</v>
+      </c>
+      <c r="E19" s="3">
+        <v>504</v>
+      </c>
+      <c r="F19" s="3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C20" s="3">
+        <v>716</v>
+      </c>
+      <c r="D20" s="3">
+        <v>10383</v>
+      </c>
+      <c r="E20" s="3">
+        <v>595</v>
+      </c>
+      <c r="F20" s="3">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>